<commit_message>
Updated the uptimes excel table
</commit_message>
<xml_diff>
--- a/up times 01dec2020 to 31may2021.xlsx
+++ b/up times 01dec2020 to 31may2021.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4B2191-5D1F-4458-974F-C9A8AF664755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDA94D0-E2D9-444D-9B46-82CA94C5EF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1770" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="1770" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>*Buoy Season cancelled due to COVID-19 epidemic delayed servicing schedule and damaged mooring line</t>
   </si>
   <si>
-    <t>163/182 (89.6)</t>
-  </si>
-  <si>
     <t>Sensors are deemed up if samples recorded &gt; 75% typical sampling day</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>**MARI Buoy Data from 12-21-2020 to 3-24-2021, latest date serviced and data downloaded</t>
+  </si>
+  <si>
+    <t>178/182 (97.8)</t>
   </si>
 </sst>
 </file>
@@ -312,6 +312,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -324,13 +331,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -619,26 +619,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="45.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.44140625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -653,7 +653,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -671,10 +671,10 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -802,13 +802,13 @@
         <v>26</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -819,15 +819,15 @@
         <v>27</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="19"/>
+        <v>31</v>
+      </c>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -837,7 +837,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>24</v>
@@ -854,7 +854,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>24</v>
@@ -871,13 +871,13 @@
         <v>27</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -888,13 +888,13 @@
         <v>27</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -905,13 +905,13 @@
         <v>27</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -949,11 +949,11 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
@@ -969,7 +969,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>